<commit_message>
🔧 Finalized validator, email, tracker, and GitHub Actions setup
</commit_message>
<xml_diff>
--- a/data/delta_report_2025-06-18.xlsx
+++ b/data/delta_report_2025-06-18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Vendor Name</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Invoice Date</t>
+          <t>Vendor</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -456,188 +456,162 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>PAN</t>
+          <t>Amount</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>HSN Code</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Taxable Value</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Total Amount</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Reason</t>
+          <t>Validation Status</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>INV002</t>
+          <t>INV-1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>XYZ Pvt Ltd</t>
+          <t>2025-06-14</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-11</t>
+          <t>Vendor 1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>07XYZDE5678G1Z5</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>XYZDE5678G</t>
-        </is>
+          <t>29ABCDE1234F01Z5</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1180</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1002</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>15500</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>18290</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Modified</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Taxable Value changed, Total Amount changed</t>
+          <t>VALID</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>INV004</t>
+          <t>INV-2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>New Vendor</t>
+          <t>2025-06-14</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-13</t>
+          <t>Vendor 2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>07NEWVE0001I1Z5</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>NEWVE0001I</t>
-        </is>
+          <t>29ABCDE1234F02Z5</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1430</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1004</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>5000</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>5900</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>New Upload</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Not found in previous file</t>
+          <t>VALID</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>INV003</t>
+          <t>INV-3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LMN Co</t>
+          <t>2025-06-14</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-12</t>
+          <t>Vendor 3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>07LMNOP9876H1Z5</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>LMNOP9876H</t>
-        </is>
+          <t>29ABCDE1234F03Z5</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1680</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1003</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>20000</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>23600</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Deleted</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Missing in current file</t>
+          <t>VALID</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>INV-4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-06-14</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Vendor 4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>29ABCDE1234F04Z5</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1930</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>VALID</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>INV-5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-06-14</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Vendor 5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>29ABCDE1234F05Z5</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2180</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>VALID</t>
         </is>
       </c>
     </row>

</xml_diff>